<commit_message>
Updated Product and Sprint Backlog in Docs
</commit_message>
<xml_diff>
--- a/Documentation/Product_Backlog.xlsx
+++ b/Documentation/Product_Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xinophilius\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xinophilius\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BABB79B-7E4B-4E3A-B59C-084C00CACA14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8C915FE-AB20-401B-976D-1D71271B7D7E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18440" yWindow="-17250" windowWidth="19810" windowHeight="14610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -526,7 +526,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -572,7 +572,7 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -595,7 +595,7 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -618,7 +618,7 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -641,7 +641,7 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -664,7 +664,7 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <v>4</v>
@@ -687,7 +687,7 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -707,7 +707,7 @@
         <v>10</v>
       </c>
       <c r="C9">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9">
         <v>4</v>
@@ -727,7 +727,7 @@
         <v>11</v>
       </c>
       <c r="C10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -747,7 +747,7 @@
         <v>12</v>
       </c>
       <c r="C11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11">
         <v>5</v>
@@ -767,7 +767,7 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12">
         <v>4</v>
@@ -787,7 +787,7 @@
         <v>14</v>
       </c>
       <c r="C13">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13">
         <v>5</v>
@@ -807,7 +807,7 @@
         <v>30</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -827,7 +827,7 @@
         <v>15</v>
       </c>
       <c r="C15">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15">
         <v>4</v>
@@ -847,7 +847,7 @@
         <v>40</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -867,7 +867,7 @@
         <v>16</v>
       </c>
       <c r="C17">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D17">
         <v>5</v>
@@ -887,7 +887,7 @@
         <v>17</v>
       </c>
       <c r="C18">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D18">
         <v>5</v>
@@ -927,7 +927,7 @@
         <v>31</v>
       </c>
       <c r="C20">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D20">
         <v>3</v>
@@ -947,7 +947,7 @@
         <v>19</v>
       </c>
       <c r="C21">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D21">
         <v>4</v>
@@ -967,7 +967,7 @@
         <v>20</v>
       </c>
       <c r="C22">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D22">
         <v>4</v>
@@ -987,7 +987,7 @@
         <v>21</v>
       </c>
       <c r="C23">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D23">
         <v>4</v>
@@ -1007,7 +1007,7 @@
         <v>22</v>
       </c>
       <c r="C24">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D24">
         <v>5</v>
@@ -1027,7 +1027,7 @@
         <v>23</v>
       </c>
       <c r="C25">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D25">
         <v>3</v>
@@ -1047,7 +1047,7 @@
         <v>24</v>
       </c>
       <c r="C26">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D26">
         <v>4</v>
@@ -1067,7 +1067,7 @@
         <v>25</v>
       </c>
       <c r="C27">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D27">
         <v>5</v>
@@ -1087,7 +1087,7 @@
         <v>26</v>
       </c>
       <c r="C28">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D28">
         <v>5</v>
@@ -1107,7 +1107,7 @@
         <v>27</v>
       </c>
       <c r="C29">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D29">
         <v>5</v>

</xml_diff>